<commit_message>
Updating the progress sheet
git-tfs-id: [http://developmentvlan:8585/tfs/vanrise.collection]$/;C55268
</commit_message>
<xml_diff>
--- a/SOM/Documents/SOM/SOM Progress.xlsx
+++ b/SOM/Documents/SOM/SOM Progress.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanrise2015\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TFS\SOM\Documents\SOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -456,9 +456,13 @@
   <autoFilter ref="A1:F53">
     <filterColumn colId="1">
       <filters>
-        <filter val="Completed"/>
         <filter val="New"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="6">
@@ -739,7 +743,7 @@
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,7 +775,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -788,7 +792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -805,7 +809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -822,7 +826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -839,12 +843,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -856,7 +860,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -870,7 +874,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -898,7 +902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -915,12 +919,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
         <v>13</v>
@@ -942,16 +946,19 @@
       <c r="C12" t="s">
         <v>13</v>
       </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
@@ -963,7 +970,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -980,12 +987,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -997,7 +1004,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>37</v>
       </c>
@@ -1021,16 +1028,19 @@
       <c r="C17" t="s">
         <v>13</v>
       </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -1042,7 +1052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>42</v>
       </c>
@@ -1069,11 +1079,14 @@
       <c r="C20" t="s">
         <v>13</v>
       </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>46</v>
       </c>
@@ -1090,7 +1103,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1104,7 +1117,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -1121,7 +1134,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>52</v>
       </c>
@@ -1138,7 +1151,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>56</v>
       </c>
@@ -1155,12 +1168,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>58</v>
       </c>
       <c r="B26" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
         <v>13</v>
@@ -1175,7 +1188,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>61</v>
       </c>
@@ -1189,12 +1202,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>86</v>
       </c>
       <c r="B28" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
         <v>13</v>
@@ -1209,7 +1222,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1223,7 +1236,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>67</v>
       </c>
@@ -1247,11 +1260,14 @@
       <c r="C31" t="s">
         <v>13</v>
       </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>71</v>
       </c>
@@ -1265,7 +1281,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -1279,7 +1295,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>74</v>
       </c>
@@ -1293,7 +1309,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1307,7 +1323,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>77</v>
       </c>
@@ -1321,7 +1337,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -1345,11 +1361,14 @@
       <c r="C38" t="s">
         <v>13</v>
       </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>84</v>
       </c>
@@ -1373,11 +1392,14 @@
       <c r="C40" t="s">
         <v>13</v>
       </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>89</v>
       </c>
@@ -1391,7 +1413,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>91</v>
       </c>
@@ -1408,7 +1430,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>93</v>
       </c>
@@ -1425,7 +1447,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>96</v>
       </c>
@@ -1442,7 +1464,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>99</v>
       </c>
@@ -1456,7 +1478,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>101</v>
       </c>
@@ -1480,11 +1502,14 @@
       <c r="C47" t="s">
         <v>13</v>
       </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -1508,6 +1533,9 @@
       <c r="C49" t="s">
         <v>13</v>
       </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>109</v>
       </c>
@@ -1522,6 +1550,9 @@
       <c r="C50" t="s">
         <v>13</v>
       </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>111</v>
       </c>
@@ -1539,6 +1570,9 @@
       <c r="C51" t="s">
         <v>13</v>
       </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>113</v>
       </c>
@@ -1546,7 +1580,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -1563,7 +1597,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>117</v>
       </c>

</xml_diff>